<commit_message>
Found reliable way to select cells from table, still needs a fair bit of tweaking though
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Test_Framework/_Tests.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Test_Framework/_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,11 +787,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
       <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="4:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="4:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8 B10:B28">
@@ -807,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clean up of test results
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Test_Framework/_Tests.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Test_Framework/_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Initialise with Invalid Config</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Arguments</t>
   </si>
   <si>
@@ -73,18 +70,12 @@
     <t>Check development account and exchange folders</t>
   </si>
   <si>
-    <t>No exception thrown</t>
-  </si>
-  <si>
     <t>200000199</t>
   </si>
   <si>
     <t>2018001812</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>201100215</t>
   </si>
   <si>
@@ -133,9 +124,6 @@
     <t>DEV</t>
   </si>
   <si>
-    <t>UAT</t>
-  </si>
-  <si>
     <t>PRD</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>\Test_Framework\Test_SearchRMNumber.xaml</t>
   </si>
   <si>
-    <t>An exception was meant to be thrown</t>
-  </si>
-  <si>
     <t>Test_Framework\Exchange\Test_GetExchangeMail.xaml</t>
   </si>
   <si>
@@ -193,55 +178,16 @@
     <t>SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Testing\Excess Mailbox Path</t>
   </si>
   <si>
-    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceRequestException: The request failed. The remote server returned an error: (503) Server Unavailable. ---&gt; System.Net.WebException: The remote server returned an error: (503) Server Unavailable._x000D_
-   at System.Net.HttpWebRequest.GetResponse()_x000D_
-   at Microsoft.Exchange.WebServices.Data.EwsHttpWebRequest.Microsoft.Exchange.WebServices.Data.IEwsHttpWebRequest.GetResponse() in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\EwsHttpWebRequest.cs:line 113_x000D_
-   at Microsoft.Exchange.WebServices.Data.ServiceRequestBase.GetEwsHttpWebResponse(IEwsHttpWebRequest request) in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\Requests\ServiceRequestBase.cs:line 821_x000D_
-   --- End of inner exception stack trace ---_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
-    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceRequestException: The request failed. The remote name could not be resolved: 'invalid.office365.com' ---&gt; System.Net.WebException: The remote name could not be resolved: 'invalid.office365.com'_x000D_
-   at System.Net.HttpWebRequest.EndGetRequestStream(IAsyncResult asyncResult, TransportContext&amp; context)_x000D_
-   at System.Net.HttpWebRequest.EndGetRequestStream(IAsyncResult asyncResult)_x000D_
-   at Microsoft.Exchange.WebServices.Data.EwsHttpWebRequest.Microsoft.Exchange.WebServices.Data.IEwsHttpWebRequest.EndGetRequestStream(IAsyncResult asyncResult) in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\EwsHttpWebRequest.cs:line 79_x000D_
-   at Microsoft.Exchange.WebServices.Data.ServiceRequestBase.EmitRequest(IEwsHttpWebRequest request) in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\Requests\ServiceRequestBase.cs:line 413_x000D_
-   at Microsoft.Exchange.WebServices.Data.ServiceRequestBase.BuildEwsHttpWebRequest() in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\Requests\ServiceRequestBase.cs:line 790_x000D_
-   --- End of inner exception stack trace ---_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
-    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceResponseException: The SMTP address has no mailbox associated with it._x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
-    <t>Should throw AppEx: System.Exception: Couldn't find Minion - Incorrect Path_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
-    <t>Should throw AppEx: System.Exception: Couldn't find Excess Mailbox Path_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
     <t>Test_Framework\Test_LoginToUniFi.xaml</t>
   </si>
   <si>
     <t>SSO_rpa00002,https://fs92rept.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Proforma-TEST-UniFi,https://fs92rept.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
   </si>
 </sst>
 </file>
@@ -599,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -632,29 +578,29 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="8" t="s">
-        <v>36</v>
+      <c r="D3" t="s">
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -662,14 +608,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -677,14 +623,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -695,115 +641,115 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -812,146 +758,160 @@
     </row>
     <row r="16" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="9"/>
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
         <v>30</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
+      <c r="D21" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="8">
-        <v>2018001377</v>
-      </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="D23" s="8">
+        <v>2018001377</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B27 B30:B37 B2:B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B12 B31:B38 B16:B28">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>
@@ -962,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,78 +949,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,274 +960,26 @@
       <c r="B6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5">
-        <v>2018001377</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="5">
-        <v>200000199</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5">
-        <v>2018001812</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="5">
-        <v>201100215</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>

</xml_diff>